<commit_message>
quick change to field mappings
</commit_message>
<xml_diff>
--- a/docs/fieldMapping.xlsx
+++ b/docs/fieldMapping.xlsx
@@ -809,7 +809,7 @@
   <dimension ref="B2:U65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,6 +1194,9 @@
       <c r="T19">
         <v>0</v>
       </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20">
@@ -1342,9 +1345,6 @@
       </c>
       <c r="T23">
         <v>0</v>
-      </c>
-      <c r="U23">
-        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Game Logic functionally working
</commit_message>
<xml_diff>
--- a/docs/fieldMapping.xlsx
+++ b/docs/fieldMapping.xlsx
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24">
         <v>2</v>

</xml_diff>

<commit_message>
commented out test buttons
</commit_message>
<xml_diff>
--- a/docs/fieldMapping.xlsx
+++ b/docs/fieldMapping.xlsx
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,6 +1640,9 @@
       </c>
       <c r="E31">
         <v>14</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
       </c>
       <c r="J31">
         <v>16</v>

</xml_diff>